<commit_message>
all export type has been completed
</commit_message>
<xml_diff>
--- a/测试.xlsx
+++ b/测试.xlsx
@@ -10,12 +10,13 @@
     <sheet name="2020年&quot;个人成长基金&quot;项目收支表" sheetId="3" r:id="rId3"/>
     <sheet name="2020年度&quot;个人成长基金&quot;项目收支统计表" sheetId="4" r:id="rId4"/>
     <sheet name="2020年3月凭证列表" sheetId="5" r:id="rId5"/>
+    <sheet name="2020年3月“个人成长基金”项目凭证详情" sheetId="6" r:id="rId6"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
   <si>
     <t>2020年度资金表</t>
   </si>
@@ -177,6 +178,12 @@
   </si>
   <si>
     <t>没事</t>
+  </si>
+  <si>
+    <t>2020年3月“个人成长基金”项目凭证详情</t>
+  </si>
+  <si>
+    <t>类型</t>
   </si>
 </sst>
 </file>
@@ -1902,4 +1909,84 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K3"/>
+  <sheetViews>
+    <sheetView showGridLines="1" workbookViewId="0" rightToLeft="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="2" max="2" width="25" customWidth="1"/>
+    <col min="5" max="5" width="40" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="4"/>
+      <c r="B2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="4" t="n">
+        <v>50</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F3" s="4" t="n">
+        <v>50</v>
+      </c>
+      <c r="G3" s="4" t="n">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A3:A3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>